<commit_message>
Handling more than one digit number
</commit_message>
<xml_diff>
--- a/New Microsoft Excel Worksheet.xlsx
+++ b/New Microsoft Excel Worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ADVANSYS\Transcation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C74CE26B-3C01-479C-BD1F-CDF8C0863DE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6C481F4-D3E1-4E8A-B018-E00D67408439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,15 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>ID</t>
   </si>
   <si>
     <t>Transcations</t>
-  </si>
-  <si>
-    <t>e</t>
   </si>
 </sst>
 </file>
@@ -351,10 +348,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -380,15 +377,15 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>2</v>
+      <c r="B4">
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -397,6 +394,30 @@
       </c>
       <c r="B5">
         <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>